<commit_message>
time card and backlog update
</commit_message>
<xml_diff>
--- a/Time Chart.xlsx
+++ b/Time Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="84" windowWidth="16260" windowHeight="5856" activeTab="1"/>
+    <workbookView xWindow="384" yWindow="84" windowWidth="16260" windowHeight="5856"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="4" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Name</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Week</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
@@ -143,11 +146,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="196657152"/>
-        <c:axId val="196658688"/>
+        <c:axId val="194760704"/>
+        <c:axId val="194762240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="196657152"/>
+        <c:axId val="194760704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -156,7 +159,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196658688"/>
+        <c:crossAx val="194762240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -164,7 +167,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="196658688"/>
+        <c:axId val="194762240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -194,7 +197,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="196657152"/>
+        <c:crossAx val="194760704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -356,6 +359,12 @@
                 <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -456,6 +465,12 @@
                 <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -556,6 +571,12 @@
                 <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -656,6 +677,12 @@
                 <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -756,6 +783,12 @@
                 <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -856,6 +889,12 @@
                 <c:pt idx="4">
                   <c:v>3</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -942,7 +981,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>70</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -959,11 +998,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="197254144"/>
-        <c:axId val="197268224"/>
+        <c:axId val="194632704"/>
+        <c:axId val="194646784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="197254144"/>
+        <c:axId val="194632704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -974,7 +1013,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197268224"/>
+        <c:crossAx val="194646784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -982,7 +1021,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="197268224"/>
+        <c:axId val="194646784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="12"/>
@@ -994,7 +1033,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="197254144"/>
+        <c:crossAx val="194632704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1025,7 +1064,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1521,10 +1560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1532,12 +1571,15 @@
     <col min="1" max="1" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="R1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1590,7 +1632,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1609,8 +1651,18 @@
       <c r="F3">
         <v>3</v>
       </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="R3">
+        <f>SUM(B3:Q3)</f>
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1629,8 +1681,18 @@
       <c r="F4">
         <v>3</v>
       </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>6</v>
+      </c>
+      <c r="R4">
+        <f>SUM(B4:Q4)</f>
+        <v>22</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1649,8 +1711,18 @@
       <c r="F5">
         <v>3</v>
       </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="R5">
+        <f>SUM(B5:Q5)</f>
+        <v>22</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1669,8 +1741,18 @@
       <c r="F6">
         <v>3</v>
       </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="R6">
+        <f>SUM(B6:Q6)</f>
+        <v>19</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1689,8 +1771,18 @@
       <c r="F7">
         <v>3</v>
       </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>6</v>
+      </c>
+      <c r="R7">
+        <f xml:space="preserve"> SUM(B7:Q7)</f>
+        <v>21</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1709,14 +1801,24 @@
       <c r="F8">
         <v>3</v>
       </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="R8">
+        <f>SUM(B8:Q8)</f>
+        <v>21</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9">
         <f xml:space="preserve"> SUM(B3:Q8)</f>
-        <v>70</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>